<commit_message>
Ignorar saltos de línea en notebooks
</commit_message>
<xml_diff>
--- a/db/Clase.xlsx
+++ b/db/Clase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PosGrado\Proyecto Titulacion\Timetabling\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74FCB8E-23E3-408A-8AD6-036B55431808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B516D2A4-E4BD-44D3-9541-BDE6B3BB4202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6CAC09B9-9E24-49B8-BB40-D925C9E2F3A4}"/>
+    <workbookView xWindow="2940" yWindow="3660" windowWidth="28785" windowHeight="15345" xr2:uid="{6CAC09B9-9E24-49B8-BB40-D925C9E2F3A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>